<commit_message>
fix TAL GWP breakdown parameter; update 3-HP TRY for larger ferm space
</commit_message>
<xml_diff>
--- a/biorefineries/TAL/analyses/results/TAL_2024/full/baseline_A.xlsx
+++ b/biorefineries/TAL/analyses/results/TAL_2024/full/baseline_A.xlsx
@@ -2200,7 +2200,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4.427743854815509</v>
+        <v>4.427743854815507</v>
       </c>
       <c r="C4" t="n">
         <v>14.70674838170381</v>
@@ -2209,7 +2209,7 @@
         <v>0.910149435743323</v>
       </c>
       <c r="E4" t="n">
-        <v>4.864853705259238</v>
+        <v>4.864853705259232</v>
       </c>
       <c r="F4" t="n">
         <v>13.38533874122675</v>
@@ -2218,10 +2218,10 @@
         <v>0.7191414765597666</v>
       </c>
       <c r="H4" t="n">
-        <v>290.0212508371825</v>
+        <v>290.0212508371824</v>
       </c>
       <c r="I4" t="n">
-        <v>159.6686604967904</v>
+        <v>159.6686604967903</v>
       </c>
       <c r="J4" t="n">
         <v>33.38533180189852</v>
@@ -2233,13 +2233,13 @@
         <v>30.30511281195226</v>
       </c>
       <c r="M4" t="n">
-        <v>65.11771477140697</v>
+        <v>65.11771477140688</v>
       </c>
       <c r="N4" t="n">
-        <v>16.33161352255113</v>
+        <v>16.33161352255112</v>
       </c>
       <c r="O4" t="n">
-        <v>-2.747401595115662e-08</v>
+        <v>-7.031485438346863e-07</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -2359,10 +2359,10 @@
         <v>0</v>
       </c>
       <c r="BC4" t="n">
-        <v>55.34654587216853</v>
+        <v>55.34654587216855</v>
       </c>
       <c r="BD4" t="n">
-        <v>35.4475038063432</v>
+        <v>35.44750380634321</v>
       </c>
       <c r="BE4" t="n">
         <v>274.7102660794025</v>
@@ -2599,7 +2599,7 @@
         <v>0.00365139735511587</v>
       </c>
       <c r="EE4" t="n">
-        <v>0.3274272947531236</v>
+        <v>0.3274272947531235</v>
       </c>
       <c r="EF4" t="n">
         <v>0</v>
@@ -2647,7 +2647,7 @@
         <v>0.1514251500899552</v>
       </c>
       <c r="EU4" t="n">
-        <v>0.0969824493941715</v>
+        <v>0.09698244939417154</v>
       </c>
       <c r="EV4" t="n">
         <v>0.7515924005158734</v>
@@ -2872,7 +2872,7 @@
         <v>-9.399224785514415</v>
       </c>
       <c r="HR4" t="n">
-        <v>24.4372968911415</v>
+        <v>1.714382189571905</v>
       </c>
       <c r="HS4" t="n">
         <v>5.856456505495864</v>
@@ -2947,7 +2947,7 @@
         <v>-0.711807117986905</v>
       </c>
       <c r="IQ4" t="n">
-        <v>1.850646438234085</v>
+        <v>0.1298308608777964</v>
       </c>
       <c r="IR4" t="n">
         <v>0.4435118344246007</v>
@@ -3020,7 +3020,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4.42779899040535</v>
+        <v>4.427798990405352</v>
       </c>
       <c r="C5" t="n">
         <v>14.706580264477</v>
@@ -3029,7 +3029,7 @@
         <v>0.9101494398856455</v>
       </c>
       <c r="E5" t="n">
-        <v>4.864914261730109</v>
+        <v>4.864914261730114</v>
       </c>
       <c r="F5" t="n">
         <v>13.38518579034703</v>
@@ -3053,13 +3053,13 @@
         <v>30.3050717794609</v>
       </c>
       <c r="M5" t="n">
-        <v>65.11778124736648</v>
+        <v>65.11778124736654</v>
       </c>
       <c r="N5" t="n">
         <v>16.33164880685249</v>
       </c>
       <c r="O5" t="n">
-        <v>-6.081536412239075e-07</v>
+        <v>-2.002343535423279e-08</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -3179,7 +3179,7 @@
         <v>0</v>
       </c>
       <c r="BC5" t="n">
-        <v>55.34622102282856</v>
+        <v>55.34622102282853</v>
       </c>
       <c r="BD5" t="n">
         <v>35.44714370770919</v>
@@ -3464,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="ET5" t="n">
-        <v>0.1514260027085009</v>
+        <v>0.1514260027085008</v>
       </c>
       <c r="EU5" t="n">
         <v>0.09698257947689364</v>
@@ -3602,16 +3602,16 @@
         <v>0.4288660504031421</v>
       </c>
       <c r="GN5" t="n">
-        <v>0.0004101909841451006</v>
+        <v>0.0004101909841451007</v>
       </c>
       <c r="GO5" t="n">
-        <v>0.05702448181567569</v>
+        <v>0.0570244818156757</v>
       </c>
       <c r="GP5" t="n">
-        <v>0.1003615077973585</v>
+        <v>0.1003615077973586</v>
       </c>
       <c r="GQ5" t="n">
-        <v>0.06632047931571887</v>
+        <v>0.06632047931571888</v>
       </c>
       <c r="GR5" t="n">
         <v>0</v>
@@ -3620,13 +3620,13 @@
         <v>0</v>
       </c>
       <c r="GT5" t="n">
-        <v>7.439444289531757e-06</v>
+        <v>7.439444289531758e-06</v>
       </c>
       <c r="GU5" t="n">
-        <v>7.500344594240784e-06</v>
+        <v>7.500344594240785e-06</v>
       </c>
       <c r="GV5" t="n">
-        <v>6.773271466802411e-07</v>
+        <v>6.773271466802412e-07</v>
       </c>
       <c r="GW5" t="n">
         <v>0</v>
@@ -3692,7 +3692,7 @@
         <v>-9.399211808211488</v>
       </c>
       <c r="HR5" t="n">
-        <v>24.43731027787893</v>
+        <v>1.714371296905782</v>
       </c>
       <c r="HS5" t="n">
         <v>5.856459122159591</v>
@@ -3767,7 +3767,7 @@
         <v>-0.7118052664881498</v>
       </c>
       <c r="IQ5" t="n">
-        <v>1.850645193398308</v>
+        <v>0.1298298775209597</v>
       </c>
       <c r="IR5" t="n">
         <v>0.4435114913022679</v>

</xml_diff>